<commit_message>
typos in salary negotiation worksheet
</commit_message>
<xml_diff>
--- a/extras/FearlessSalaryNegotiation_Extras_Chapter4-SalaryNegotiation_Worksheet v01.xlsx
+++ b/extras/FearlessSalaryNegotiation_Extras_Chapter4-SalaryNegotiation_Worksheet v01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="380" windowWidth="24000" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="3700" yWindow="500" windowWidth="24000" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Getting started" sheetId="3" r:id="rId1"/>
@@ -797,7 +797,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>For each increment, list your second option (assuming they cannot accomodate your first option).</a:t>
+            <a:t>For each increment, list your second option (assuming they cannot accommodate your first option).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -807,7 +807,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>For each increment, list your third option (assuming they cannot accomodate your second option).</a:t>
+            <a:t>For each increment, list your third option (assuming they cannot accommodate your second option).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2490,7 +2490,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>If they can accomodate your first option ("We can do $60,000."), then you're finished.</a:t>
+            <a:t>If they can accommodate your first option ("We can do $60,000."), then you're finished.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2500,7 +2500,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>If they cannot accomodate your first option, you move to your second option: "I would be more comfortable at $58,000 if we can also find a way to add an additional week of paid vacation each year."</a:t>
+            <a:t>If they cannot accommodate your first option, you move to your second option: "I would be more comfortable at $58,000 if we can also find a way to add an additional week of paid vacation each year."</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2520,7 +2520,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>If they cannot accomodate your second option, you move to your third option: "I understand you cannot offer an additional week of vacation, but is there any way you can help cover the cost of my $250 monthly office lease?".</a:t>
+            <a:t>If they cannot accommodate your second option, you move to your third option: "I understand you cannot offer an additional week of vacation, but is there any way you can help cover the cost of my $250 monthly office lease?".</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2556,7 +2556,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0"/>
-            <a:t>In this example, they were able to do $58,000 base salary and offered an extra week of vacation in addition to your base salary (your second option). Meaning they offered $58,000, you responded with your first option of $60,000, the could not do that, so you responded with your second option of "What about an extra week of vacation?" and they were able to accomodate. So their final offer is $58,000 with an extra week of vacation and that should be enough to get you on board given your original script.</a:t>
+            <a:t>In this example, they were able to do $58,000 base salary and offered an extra week of vacation in addition to your base salary (your second option). Meaning they offered $58,000, you responded with your first option of $60,000, the could not do that, so you responded with your second option of "What about an extra week of vacation?" and they were able to accommodate . So their final offer is $58,000 with an extra week of vacation and that should be enough to get you on board given your original script.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3364,7 +3364,7 @@
   <dimension ref="C10:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3597,7 +3597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A20:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>